<commit_message>
refonte import - conversion currency
</commit_message>
<xml_diff>
--- a/data/xls/IKMS Transfert Mali Anacarde.xlsx
+++ b/data/xls/IKMS Transfert Mali Anacarde.xlsx
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="115">
-  <si>
-    <t xml:space="preserve">Here you define the studied value chain key characteristics, in order to match economic, social and ACV studies part</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="114">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -385,7 +382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -407,12 +404,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -477,11 +468,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,8 +502,8 @@
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -535,295 +526,295 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>966470.4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>241920</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>1578034.68208093</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>27452.25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>538214.4140625</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>10857.7292413088</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>16000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -846,19 +837,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,13 +857,13 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>2833493959.98916</v>
@@ -883,13 +874,13 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>0</v>
@@ -900,13 +891,13 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>213760000</v>
@@ -917,13 +908,13 @@
         <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>4435200</v>
@@ -934,13 +925,13 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>2822400</v>
@@ -951,13 +942,13 @@
         <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>2833333.359375</v>
@@ -968,13 +959,13 @@
         <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>0</v>
@@ -985,13 +976,13 @@
         <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0</v>
@@ -1002,13 +993,13 @@
         <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -1019,13 +1010,13 @@
         <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -1036,13 +1027,13 @@
         <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>1739884393.06358</v>
@@ -1053,13 +1044,13 @@
         <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>270165000</v>
@@ -1070,13 +1061,13 @@
         <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>1067744000</v>
@@ -1087,13 +1078,13 @@
         <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>27638553600</v>
@@ -1104,13 +1095,13 @@
         <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>29482790400</v>
@@ -1121,13 +1112,13 @@
         <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>19730000</v>
@@ -1138,13 +1129,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>0</v>
@@ -1155,13 +1146,13 @@
         <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E19" s="2" t="n">
         <v>0</v>
@@ -1172,13 +1163,13 @@
         <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>0</v>
@@ -1189,13 +1180,13 @@
         <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
@@ -1206,13 +1197,13 @@
         <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -1223,13 +1214,13 @@
         <v>48</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E23" s="2" t="n">
         <v>0</v>
@@ -1240,13 +1231,13 @@
         <v>49</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>0</v>
@@ -1257,13 +1248,13 @@
         <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E25" s="2" t="n">
         <v>0</v>
@@ -1274,13 +1265,13 @@
         <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>0</v>
@@ -1291,13 +1282,13 @@
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>0</v>
@@ -1308,13 +1299,13 @@
         <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>0</v>
@@ -1325,13 +1316,13 @@
         <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E29" s="2" t="n">
         <v>0</v>
@@ -1342,13 +1333,13 @@
         <v>55</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="2" t="n">
         <v>0</v>
@@ -1359,13 +1350,13 @@
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E31" s="2" t="n">
         <v>0</v>
@@ -1376,13 +1367,13 @@
         <v>47</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E32" s="2" t="n">
         <v>0</v>
@@ -1393,13 +1384,13 @@
         <v>48</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E33" s="2" t="n">
         <v>0</v>
@@ -1410,13 +1401,13 @@
         <v>49</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E34" s="2" t="n">
         <v>0</v>
@@ -1427,13 +1418,13 @@
         <v>50</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E35" s="2" t="n">
         <v>0</v>
@@ -1444,13 +1435,13 @@
         <v>51</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E36" s="2" t="n">
         <v>0</v>
@@ -1461,13 +1452,13 @@
         <v>52</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="2" t="n">
         <v>0</v>
@@ -1478,13 +1469,13 @@
         <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E38" s="2" t="n">
         <v>0</v>
@@ -1495,13 +1486,13 @@
         <v>54</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E39" s="2" t="n">
         <v>0</v>
@@ -1512,13 +1503,13 @@
         <v>55</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E40" s="2" t="n">
         <v>0</v>
@@ -1529,13 +1520,13 @@
         <v>56</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E41" s="2" t="n">
         <v>0</v>
@@ -1546,13 +1537,13 @@
         <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E42" s="2" t="n">
         <v>21143675982.2074</v>
@@ -1563,13 +1554,13 @@
         <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E43" s="2" t="n">
         <v>10108875</v>
@@ -1580,13 +1571,13 @@
         <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E44" s="2" t="n">
         <v>-306144000</v>
@@ -1597,13 +1588,13 @@
         <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E45" s="2" t="n">
         <v>460051200</v>
@@ -1614,13 +1605,13 @@
         <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E46" s="2" t="n">
         <v>71164800</v>
@@ -1631,13 +1622,13 @@
         <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E47" s="2" t="n">
         <v>36666.640625</v>
@@ -1648,13 +1639,13 @@
         <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" s="2" t="n">
         <v>0</v>
@@ -1665,13 +1656,13 @@
         <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E49" s="2" t="n">
         <v>0</v>
@@ -1682,13 +1673,13 @@
         <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50" s="2" t="n">
         <v>0</v>
@@ -1699,13 +1690,13 @@
         <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E51" s="2" t="n">
         <v>0</v>
@@ -1716,13 +1707,13 @@
         <v>47</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E52" s="2" t="n">
         <v>28564800000</v>
@@ -1733,13 +1724,13 @@
         <v>48</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E53" s="2" t="n">
         <v>294000000</v>
@@ -1750,13 +1741,13 @@
         <v>49</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E54" s="2" t="n">
         <v>1344000000</v>
@@ -1767,13 +1758,13 @@
         <v>50</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E55" s="2" t="n">
         <v>28224000000</v>
@@ -1784,13 +1775,13 @@
         <v>51</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E56" s="2" t="n">
         <v>30240000000</v>
@@ -1801,13 +1792,13 @@
         <v>52</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E57" s="2" t="n">
         <v>30600000</v>
@@ -1818,13 +1809,13 @@
         <v>53</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E58" s="2" t="n">
         <v>0</v>
@@ -1835,13 +1826,13 @@
         <v>54</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E59" s="2" t="n">
         <v>0</v>
@@ -1852,13 +1843,13 @@
         <v>55</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E60" s="2" t="n">
         <v>0</v>
@@ -1869,13 +1860,13 @@
         <v>56</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E61" s="2" t="n">
         <v>0</v>
@@ -1886,13 +1877,13 @@
         <v>47</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E62" s="2" t="n">
         <v>0</v>
@@ -1903,13 +1894,13 @@
         <v>48</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E63" s="2" t="n">
         <v>0</v>
@@ -1920,13 +1911,13 @@
         <v>49</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E64" s="2" t="n">
         <v>0</v>
@@ -1937,13 +1928,13 @@
         <v>50</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E65" s="2" t="n">
         <v>0</v>
@@ -1954,13 +1945,13 @@
         <v>51</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E66" s="2" t="n">
         <v>0</v>
@@ -1971,13 +1962,13 @@
         <v>52</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E67" s="2" t="n">
         <v>0</v>
@@ -1988,13 +1979,13 @@
         <v>53</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E68" s="2" t="n">
         <v>0</v>
@@ -2005,13 +1996,13 @@
         <v>54</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E69" s="2" t="n">
         <v>0</v>
@@ -2022,13 +2013,13 @@
         <v>55</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E70" s="2" t="n">
         <v>0</v>
@@ -2039,13 +2030,13 @@
         <v>56</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E71" s="2" t="n">
         <v>0</v>
@@ -2056,13 +2047,13 @@
         <v>47</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E72" s="2" t="n">
         <v>0</v>
@@ -2073,13 +2064,13 @@
         <v>48</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E73" s="2" t="n">
         <v>0</v>
@@ -2090,13 +2081,13 @@
         <v>49</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E74" s="2" t="n">
         <v>0</v>
@@ -2107,13 +2098,13 @@
         <v>50</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E75" s="2" t="n">
         <v>0</v>
@@ -2124,13 +2115,13 @@
         <v>51</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E76" s="2" t="n">
         <v>62899200</v>
@@ -2141,13 +2132,13 @@
         <v>52</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E77" s="2" t="n">
         <v>0</v>
@@ -2158,13 +2149,13 @@
         <v>53</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E78" s="2" t="n">
         <v>0</v>
@@ -2175,13 +2166,13 @@
         <v>54</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E79" s="2" t="n">
         <v>0</v>
@@ -2192,13 +2183,13 @@
         <v>55</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E80" s="2" t="n">
         <v>0</v>
@@ -2209,13 +2200,13 @@
         <v>56</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E81" s="2" t="n">
         <v>0</v>
@@ -2226,13 +2217,13 @@
         <v>47</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E82" s="2" t="n">
         <v>2367052023.12139</v>
@@ -2243,13 +2234,13 @@
         <v>48</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E83" s="2" t="n">
         <v>13726125</v>
@@ -2260,13 +2251,13 @@
         <v>49</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E84" s="2" t="n">
         <v>368640000</v>
@@ -2277,13 +2268,13 @@
         <v>50</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E85" s="2" t="n">
         <v>120960000</v>
@@ -2294,13 +2285,13 @@
         <v>51</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E86" s="2" t="n">
         <v>483235200</v>
@@ -2311,13 +2302,13 @@
         <v>52</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E87" s="2" t="n">
         <v>8000000</v>
@@ -2328,13 +2319,13 @@
         <v>53</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E88" s="2" t="n">
         <v>0</v>
@@ -2345,13 +2336,13 @@
         <v>54</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E89" s="2" t="n">
         <v>0</v>
@@ -2362,13 +2353,13 @@
         <v>55</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E90" s="2" t="n">
         <v>0</v>
@@ -2379,13 +2370,13 @@
         <v>56</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E91" s="2" t="n">
         <v>0</v>
@@ -2393,8 +2384,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2416,8 +2407,8 @@
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2433,186 +2424,188 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.39453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="21.40234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="2" t="n">
+        <v>2014</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>2014</v>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>42000000</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>80000</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>42000000</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="2" t="n">
-        <v>80000</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -2620,29 +2613,29 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2653,7 +2646,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -2664,44 +2657,34 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2724,13 +2707,12 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A8:E8"/>
+  <mergeCells count="1">
+    <mergeCell ref="A7:E7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2753,46 +2735,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2815,13 +2797,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,10 +2811,10 @@
         <v>47</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,10 +2822,10 @@
         <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,10 +2833,10 @@
         <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,10 +2844,10 @@
         <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,10 +2855,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,10 +2866,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2895,10 +2877,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,10 +2888,10 @@
         <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,10 +2899,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,16 +2910,16 @@
         <v>56</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2960,22 +2942,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2998,34 +2980,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3033,16 +3015,16 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>336000</v>
@@ -3054,7 +3036,7 @@
         <v>680</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3062,16 +3044,16 @@
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>1344000</v>
@@ -3083,7 +3065,7 @@
         <v>680</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3091,16 +3073,16 @@
         <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>40320000</v>
@@ -3112,7 +3094,7 @@
         <v>680</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,16 +3102,16 @@
         <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>80000</v>
@@ -3141,7 +3123,7 @@
         <v>60</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3149,16 +3131,16 @@
         <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>73500</v>
@@ -3170,7 +3152,7 @@
         <v>4000</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3178,16 +3160,16 @@
         <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>268800</v>
@@ -3199,7 +3181,7 @@
         <v>5000</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3207,16 +3189,16 @@
         <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>40320000</v>
@@ -3228,7 +3210,7 @@
         <v>700</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3236,16 +3218,16 @@
         <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>40320000</v>
@@ -3257,7 +3239,7 @@
         <v>750</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3265,16 +3247,16 @@
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>40000</v>
@@ -3286,13 +3268,13 @@
         <v>765</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3315,25 +3297,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3341,7 +3323,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>33694.3441636582</v>
@@ -3364,7 +3346,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
@@ -3387,7 +3369,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>25</v>
@@ -3410,7 +3392,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
@@ -3433,7 +3415,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
@@ -3456,7 +3438,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
@@ -3476,8 +3458,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3500,19 +3482,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3535,13 +3517,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,7 +3531,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>21143675982.2074</v>
@@ -3560,7 +3542,7 @@
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>10108875</v>
@@ -3571,7 +3553,7 @@
         <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>-306144000</v>
@@ -3582,7 +3564,7 @@
         <v>50</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>460051200</v>
@@ -3593,7 +3575,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>71164800</v>
@@ -3604,7 +3586,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>36666.640625</v>
@@ -3612,7 +3594,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>0</v>
@@ -3620,7 +3602,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>3057344893.34854</v>
@@ -3628,7 +3610,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>3361613348.12139</v>
@@ -3636,7 +3618,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
@@ -3644,7 +3626,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>62899200</v>
@@ -3652,8 +3634,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>